<commit_message>
changed diffusion parameters so that Unloading can contribute to growth and not be retained in phloem
</commit_message>
<xml_diff>
--- a/test/inputs/Scenario_142.xlsx
+++ b/test/inputs/Scenario_142.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tigerault\package\Wheat-BRIDGES\test\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71242072-7265-46DD-8924-30BAD604E0B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4083C33-8130-4EAB-A308-4329C3ADFCE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2634,13 +2634,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F200"/>
+  <dimension ref="A1:G200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E97" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F115" sqref="F115"/>
+      <selection pane="bottomRight" activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4030,7 +4030,7 @@
         <v>1453890.8941884842</v>
       </c>
       <c r="E66" s="88">
-        <f t="shared" ref="E66:E129" si="1">D66</f>
+        <f t="shared" ref="E66:G129" si="1">D66</f>
         <v>1453890.8941884842</v>
       </c>
       <c r="F66" s="81">
@@ -5003,7 +5003,7 @@
         <v>21600</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="23" t="s">
         <v>400</v>
       </c>
@@ -5024,7 +5024,7 @@
         <v>43200</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="13" t="s">
         <v>61</v>
       </c>
@@ -5045,7 +5045,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="13" t="s">
         <v>62</v>
       </c>
@@ -5066,7 +5066,7 @@
         <v>2.0833333333333335E-4</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="13" t="s">
         <v>63</v>
       </c>
@@ -5087,7 +5087,7 @@
         <v>5.7899999999999998E-7</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="13" t="s">
         <v>64</v>
       </c>
@@ -5108,7 +5108,7 @@
         <v>2.0833333333333335E-4</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="13" t="s">
         <v>459</v>
       </c>
@@ -5129,7 +5129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="13" t="s">
         <v>461</v>
       </c>
@@ -5150,7 +5150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="71" t="s">
         <v>447</v>
       </c>
@@ -5170,7 +5170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="71" t="s">
         <v>67</v>
       </c>
@@ -5190,7 +5190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="71" t="s">
         <v>455</v>
       </c>
@@ -5212,7 +5212,7 @@
         <v>False</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="21" t="s">
         <v>66</v>
       </c>
@@ -5223,17 +5223,20 @@
         <v>202</v>
       </c>
       <c r="D123" s="60">
-        <v>1.0000000000000001E-5</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="E123" s="88">
         <f t="shared" si="1"/>
-        <v>1.0000000000000001E-5</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="F123" s="86">
+        <v>0.05</v>
+      </c>
+      <c r="G123" s="60">
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="21" t="s">
         <v>444</v>
       </c>
@@ -5254,7 +5257,7 @@
         <v>4.9999999999999999E-13</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="21" t="s">
         <v>231</v>
       </c>
@@ -5275,7 +5278,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="21" t="s">
         <v>232</v>
       </c>
@@ -5296,7 +5299,7 @@
         <v>-0.04</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="21" t="s">
         <v>233</v>
       </c>
@@ -5317,7 +5320,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="21" t="s">
         <v>234</v>
       </c>
@@ -5674,7 +5677,7 @@
         <v>4.0000000000000003E-5</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="13" t="s">
         <v>73</v>
       </c>
@@ -5695,7 +5698,7 @@
         <v>5.8333333333333335E-9</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="13" t="s">
         <v>243</v>
       </c>
@@ -5716,7 +5719,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="13" t="s">
         <v>244</v>
       </c>
@@ -5737,7 +5740,7 @@
         <v>-0.06</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="13" t="s">
         <v>245</v>
       </c>
@@ -5758,7 +5761,7 @@
         <v>0.89100000000000001</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="13" t="s">
         <v>246</v>
       </c>
@@ -5779,7 +5782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="13" t="s">
         <v>74</v>
       </c>
@@ -5800,7 +5803,7 @@
         <v>4.0000000000000003E-5</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="9" t="s">
         <v>75</v>
       </c>
@@ -5821,7 +5824,7 @@
         <v>4.0000000000000001E-8</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="9" t="s">
         <v>221</v>
       </c>
@@ -5842,7 +5845,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="9" t="s">
         <v>222</v>
       </c>
@@ -5863,7 +5866,7 @@
         <v>-4.4200000000000003E-2</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="9" t="s">
         <v>223</v>
       </c>
@@ -5884,7 +5887,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="9" t="s">
         <v>224</v>
       </c>
@@ -5905,7 +5908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="9" t="s">
         <v>76</v>
       </c>
@@ -5926,7 +5929,7 @@
         <v>2.7799999999999998E-4</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="25" t="s">
         <v>78</v>
       </c>
@@ -5944,11 +5947,15 @@
         <v>6.3200000000000001E-3</v>
       </c>
       <c r="F157" s="87">
+        <f>0.00000001/2000</f>
+        <v>5.0000000000000005E-12</v>
+      </c>
+      <c r="G157" s="87">
         <f>0.0000001/2000</f>
         <v>4.9999999999999995E-11</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="25" t="s">
         <v>248</v>
       </c>
@@ -5969,7 +5976,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="25" t="s">
         <v>249</v>
       </c>
@@ -5990,7 +5997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="25" t="s">
         <v>250</v>
       </c>
@@ -6984,7 +6991,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F157">
+  <conditionalFormatting sqref="F157:G157">
     <cfRule type="colorScale" priority="211">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>